<commit_message>
change code and results
</commit_message>
<xml_diff>
--- a/tables/diff.eigen.rank.xlsx
+++ b/tables/diff.eigen.rank.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ataka\Documents\rewiring\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFA63B6-49DF-43C8-AB3F-F89677926D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93A8AF4-DCDC-4678-AD36-3ED727716FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,6 +18,12 @@
     <sheet name="diff.rank.MFP.CCR.AL" sheetId="3" r:id="rId3"/>
     <sheet name="diff.rank.MFP.ICR.AL" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'diff.rank.Blood.CCR.AL'!$A$1:$E$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'diff.rank.Blood.ICR.AL'!$A$1:$E$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'diff.rank.MFP.CCR.AL'!$A$1:$E$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'diff.rank.MFP.ICR.AL'!$A$1:$E$19</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -538,8 +544,373 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>75</v>
+      </c>
+      <c r="C2">
+        <v>49</v>
+      </c>
+      <c r="D2">
+        <v>26</v>
+      </c>
+      <c r="E2">
+        <v>1.9054942247570501</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>47</v>
+      </c>
+      <c r="C3">
+        <v>22</v>
+      </c>
+      <c r="D3">
+        <v>25</v>
+      </c>
+      <c r="E3">
+        <v>1.82936535590868</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <v>71</v>
+      </c>
+      <c r="C4">
+        <v>53</v>
+      </c>
+      <c r="D4">
+        <v>18</v>
+      </c>
+      <c r="E4">
+        <v>1.2964632739700599</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <v>57</v>
+      </c>
+      <c r="C5">
+        <v>40</v>
+      </c>
+      <c r="D5">
+        <v>17</v>
+      </c>
+      <c r="E5">
+        <v>1.22033440512169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6">
+        <v>62</v>
+      </c>
+      <c r="C6">
+        <v>45</v>
+      </c>
+      <c r="D6">
+        <v>17</v>
+      </c>
+      <c r="E6">
+        <v>1.22033440512169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>36</v>
+      </c>
+      <c r="C7">
+        <v>20</v>
+      </c>
+      <c r="D7">
+        <v>16</v>
+      </c>
+      <c r="E7">
+        <v>1.1442055362733199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>64</v>
+      </c>
+      <c r="C8">
+        <v>48</v>
+      </c>
+      <c r="D8">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>1.1442055362733199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>15</v>
+      </c>
+      <c r="E9">
+        <v>1.06807666742494</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>40</v>
+      </c>
+      <c r="C10">
+        <v>25</v>
+      </c>
+      <c r="D10">
+        <v>15</v>
+      </c>
+      <c r="E10">
+        <v>1.06807666742494</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>49</v>
+      </c>
+      <c r="C11">
+        <v>34</v>
+      </c>
+      <c r="D11">
+        <v>15</v>
+      </c>
+      <c r="E11">
+        <v>1.06807666742494</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12">
+        <v>72</v>
+      </c>
+      <c r="C12">
+        <v>57</v>
+      </c>
+      <c r="D12">
+        <v>15</v>
+      </c>
+      <c r="E12">
+        <v>1.06807666742494</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>19</v>
+      </c>
+      <c r="D13">
+        <v>-17</v>
+      </c>
+      <c r="E13">
+        <v>-1.36804713572301</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>27</v>
+      </c>
+      <c r="D14">
+        <v>-17</v>
+      </c>
+      <c r="E14">
+        <v>-1.36804713572301</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <v>32</v>
+      </c>
+      <c r="D15">
+        <v>-17</v>
+      </c>
+      <c r="E15">
+        <v>-1.36804713572301</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>34</v>
+      </c>
+      <c r="C16">
+        <v>51</v>
+      </c>
+      <c r="D16">
+        <v>-17</v>
+      </c>
+      <c r="E16">
+        <v>-1.36804713572301</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>37</v>
+      </c>
+      <c r="C17">
+        <v>55</v>
+      </c>
+      <c r="D17">
+        <v>-18</v>
+      </c>
+      <c r="E17">
+        <v>-1.4441760045713901</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>38</v>
+      </c>
+      <c r="D18">
+        <v>-21</v>
+      </c>
+      <c r="E18">
+        <v>-1.6725626111165099</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <v>59</v>
+      </c>
+      <c r="D19">
+        <v>-43</v>
+      </c>
+      <c r="E19">
+        <v>-3.3473977257807301</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>14</v>
+      </c>
+      <c r="C20">
+        <v>58</v>
+      </c>
+      <c r="D20">
+        <v>-44</v>
+      </c>
+      <c r="E20">
+        <v>-3.4235265946291</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E20" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E20">
+      <sortCondition descending="1" ref="E1:E20"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1048576"/>
+      <selection activeCell="A2" sqref="A2:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -569,339 +940,344 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="C2">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="D2">
-        <v>-17</v>
+        <v>30</v>
       </c>
       <c r="E2">
-        <v>-1.36804713572301</v>
+        <v>2.2475278945887802</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="C3">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D3">
-        <v>-17</v>
+        <v>25</v>
       </c>
       <c r="E3">
-        <v>-1.36804713572301</v>
+        <v>1.8402670045988001</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B4">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C4">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="D4">
-        <v>-44</v>
+        <v>24</v>
       </c>
       <c r="E4">
-        <v>-3.4235265946291</v>
+        <v>1.7588148266008099</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B5">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="C5">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D5">
-        <v>-17</v>
+        <v>23</v>
       </c>
       <c r="E5">
-        <v>-1.36804713572301</v>
+        <v>1.6773626486028099</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="B6">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="C6">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="D6">
-        <v>-43</v>
+        <v>23</v>
       </c>
       <c r="E6">
-        <v>-3.3473977257807301</v>
+        <v>1.6773626486028099</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B7">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="C7">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="D7">
-        <v>-21</v>
+        <v>20</v>
       </c>
       <c r="E7">
-        <v>-1.6725626111165099</v>
+        <v>1.43300611460882</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B8">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="C8">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="D8">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E8">
-        <v>1.06807666742494</v>
+        <v>1.1886495806148301</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B9">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C9">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="D9">
-        <v>-17</v>
+        <v>16</v>
       </c>
       <c r="E9">
-        <v>-1.36804713572301</v>
+        <v>1.1071974026168301</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B10">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C10">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D10">
         <v>16</v>
       </c>
       <c r="E10">
-        <v>1.1442055362733199</v>
+        <v>1.1071974026168301</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="B11">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="C11">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="D11">
-        <v>-18</v>
+        <v>16</v>
       </c>
       <c r="E11">
-        <v>-1.4441760045713901</v>
+        <v>1.1071974026168301</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B12">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C12">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D12">
-        <v>15</v>
+        <v>-10</v>
       </c>
       <c r="E12">
-        <v>1.06807666742494</v>
+        <v>-1.01055922533107</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B13">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C13">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="D13">
-        <v>25</v>
+        <v>-10</v>
       </c>
       <c r="E13">
-        <v>1.82936535590868</v>
+        <v>-1.01055922533107</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="B14">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="D14">
-        <v>15</v>
+        <v>-12</v>
       </c>
       <c r="E14">
-        <v>1.06807666742494</v>
+        <v>-1.17346358132707</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="B15">
+        <v>44</v>
+      </c>
+      <c r="C15">
         <v>57</v>
       </c>
-      <c r="C15">
-        <v>40</v>
-      </c>
       <c r="D15">
-        <v>17</v>
+        <v>-13</v>
       </c>
       <c r="E15">
-        <v>1.22033440512169</v>
+        <v>-1.2549157593250599</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B16">
-        <v>62</v>
+        <v>25</v>
       </c>
       <c r="C16">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D16">
-        <v>17</v>
+        <v>-14</v>
       </c>
       <c r="E16">
-        <v>1.22033440512169</v>
+        <v>-1.3363679373230599</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B17">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="C17">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="D17">
-        <v>16</v>
+        <v>-15</v>
       </c>
       <c r="E17">
-        <v>1.1442055362733199</v>
+        <v>-1.4178201153210599</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B18">
-        <v>71</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="D18">
-        <v>18</v>
+        <v>-19</v>
       </c>
       <c r="E18">
-        <v>1.2964632739700599</v>
+        <v>-1.74362882731304</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B19">
-        <v>72</v>
+        <v>16</v>
       </c>
       <c r="C19">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="D19">
-        <v>15</v>
+        <v>-25</v>
       </c>
       <c r="E19">
-        <v>1.06807666742494</v>
+        <v>-2.2323418953010199</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B20">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="C20">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D20">
-        <v>26</v>
+        <v>-25</v>
       </c>
       <c r="E20">
-        <v>1.9054942247570501</v>
+        <v>-2.2323418953010199</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E20" xr:uid="{00000000-0001-0000-0100-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E20">
+      <sortCondition descending="1" ref="E1:E20"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E20"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1048576"/>
+      <selection sqref="A1:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -931,709 +1307,352 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="C2">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D2">
-        <v>-19</v>
+        <v>28</v>
       </c>
       <c r="E2">
-        <v>-1.74362882731304</v>
+        <v>2.0553425413552402</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="C3">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="D3">
-        <v>-15</v>
+        <v>20</v>
       </c>
       <c r="E3">
-        <v>-1.4178201153210599</v>
+        <v>1.5009069086595199</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="B4">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="C4">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D4">
-        <v>-25</v>
+        <v>20</v>
       </c>
       <c r="E4">
-        <v>-2.2323418953010199</v>
+        <v>1.5009069086595199</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B5">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="C5">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D5">
-        <v>-10</v>
+        <v>19</v>
       </c>
       <c r="E5">
-        <v>-1.01055922533107</v>
+        <v>1.4316024545725501</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="B6">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C6">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D6">
-        <v>-14</v>
+        <v>19</v>
       </c>
       <c r="E6">
-        <v>-1.3363679373230599</v>
+        <v>1.4316024545725501</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="B7">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C7">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D7">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E7">
-        <v>1.1071974026168301</v>
+        <v>1.29299354639862</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B8">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="C8">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D8">
-        <v>-25</v>
+        <v>17</v>
       </c>
       <c r="E8">
-        <v>-2.2323418953010199</v>
+        <v>1.29299354639862</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="B9">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C9">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D9">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="E9">
-        <v>1.7588148266008099</v>
+        <v>1.1543846382246901</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B10">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C10">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="D10">
-        <v>-10</v>
+        <v>14</v>
       </c>
       <c r="E10">
-        <v>-1.01055922533107</v>
+        <v>1.08508018413772</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B11">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="C11">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D11">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E11">
-        <v>1.43300611460882</v>
+        <v>1.08508018413772</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B12">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C12">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="D12">
-        <v>-13</v>
+        <v>-18</v>
       </c>
       <c r="E12">
-        <v>-1.2549157593250599</v>
+        <v>-1.1326623466451899</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B13">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="C13">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D13">
-        <v>16</v>
+        <v>-21</v>
       </c>
       <c r="E13">
-        <v>1.1071974026168301</v>
+        <v>-1.3405757089060899</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="B14">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C14">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="D14">
-        <v>25</v>
+        <v>-24</v>
       </c>
       <c r="E14">
-        <v>1.8402670045988001</v>
+        <v>-1.5484890711669901</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B15">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="C15">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D15">
-        <v>-12</v>
+        <v>-25</v>
       </c>
       <c r="E15">
-        <v>-1.17346358132707</v>
+        <v>-1.6177935252539499</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="C16">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="D16">
-        <v>23</v>
+        <v>-27</v>
       </c>
       <c r="E16">
-        <v>1.6773626486028099</v>
+        <v>-1.75640243342788</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B17">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C17">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="D17">
-        <v>16</v>
+        <v>-27</v>
       </c>
       <c r="E17">
-        <v>1.1071974026168301</v>
+        <v>-1.75640243342788</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="B18">
-        <v>62</v>
+        <v>16</v>
       </c>
       <c r="C18">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D18">
-        <v>17</v>
+        <v>-30</v>
       </c>
       <c r="E18">
-        <v>1.1886495806148301</v>
+        <v>-1.96431579568878</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B19">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="C19">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="D19">
-        <v>23</v>
+        <v>-30</v>
       </c>
       <c r="E19">
-        <v>1.6773626486028099</v>
+        <v>-1.96431579568878</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="B20">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="C20">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="D20">
-        <v>30</v>
+        <v>-32</v>
       </c>
       <c r="E20">
-        <v>2.2475278945887802</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2">
-        <v>10</v>
-      </c>
-      <c r="C2">
-        <v>37</v>
-      </c>
-      <c r="D2">
-        <v>-27</v>
-      </c>
-      <c r="E2">
-        <v>-1.75640243342788</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3">
-        <v>14</v>
-      </c>
-      <c r="C3">
-        <v>35</v>
-      </c>
-      <c r="D3">
-        <v>-21</v>
-      </c>
-      <c r="E3">
-        <v>-1.3405757089060899</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4">
-        <v>16</v>
-      </c>
-      <c r="C4">
-        <v>46</v>
-      </c>
-      <c r="D4">
-        <v>-30</v>
-      </c>
-      <c r="E4">
-        <v>-1.96431579568878</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5">
-        <v>20</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>17</v>
-      </c>
-      <c r="E5">
-        <v>1.29299354639862</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6">
-        <v>21</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
-      </c>
-      <c r="D6">
-        <v>14</v>
-      </c>
-      <c r="E6">
-        <v>1.08508018413772</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7">
-        <v>22</v>
-      </c>
-      <c r="C7">
-        <v>8</v>
-      </c>
-      <c r="D7">
-        <v>14</v>
-      </c>
-      <c r="E7">
-        <v>1.08508018413772</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8">
-        <v>23</v>
-      </c>
-      <c r="C8">
-        <v>53</v>
-      </c>
-      <c r="D8">
-        <v>-30</v>
-      </c>
-      <c r="E8">
-        <v>-1.96431579568878</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9">
-        <v>29</v>
-      </c>
-      <c r="C9">
-        <v>73</v>
-      </c>
-      <c r="D9">
-        <v>-44</v>
-      </c>
-      <c r="E9">
-        <v>-2.93457815290631</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10">
-        <v>30</v>
-      </c>
-      <c r="C10">
-        <v>55</v>
-      </c>
-      <c r="D10">
-        <v>-25</v>
-      </c>
-      <c r="E10">
-        <v>-1.6177935252539499</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>35</v>
-      </c>
-      <c r="C11">
-        <v>67</v>
-      </c>
-      <c r="D11">
-        <v>-32</v>
-      </c>
-      <c r="E11">
         <v>-2.1029247038627101</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12">
-        <v>40</v>
-      </c>
-      <c r="C12">
-        <v>64</v>
-      </c>
-      <c r="D12">
-        <v>-24</v>
-      </c>
-      <c r="E12">
-        <v>-1.5484890711669901</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13">
-        <v>41</v>
-      </c>
-      <c r="C13">
-        <v>26</v>
-      </c>
-      <c r="D13">
-        <v>15</v>
-      </c>
-      <c r="E13">
-        <v>1.1543846382246901</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14">
-        <v>45</v>
-      </c>
-      <c r="C14">
-        <v>72</v>
-      </c>
-      <c r="D14">
-        <v>-27</v>
-      </c>
-      <c r="E14">
-        <v>-1.75640243342788</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15">
-        <v>47</v>
-      </c>
-      <c r="C15">
-        <v>28</v>
-      </c>
-      <c r="D15">
-        <v>19</v>
-      </c>
-      <c r="E15">
-        <v>1.4316024545725501</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16">
-        <v>51</v>
-      </c>
-      <c r="C16">
-        <v>69</v>
-      </c>
-      <c r="D16">
-        <v>-18</v>
-      </c>
-      <c r="E16">
-        <v>-1.1326623466451899</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17">
-        <v>53</v>
-      </c>
-      <c r="C17">
-        <v>25</v>
-      </c>
-      <c r="D17">
-        <v>28</v>
-      </c>
-      <c r="E17">
-        <v>2.0553425413552402</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18">
-        <v>60</v>
-      </c>
-      <c r="C18">
-        <v>41</v>
-      </c>
-      <c r="D18">
-        <v>19</v>
-      </c>
-      <c r="E18">
-        <v>1.4316024545725501</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19">
-        <v>61</v>
-      </c>
-      <c r="C19">
-        <v>44</v>
-      </c>
-      <c r="D19">
-        <v>17</v>
-      </c>
-      <c r="E19">
-        <v>1.29299354639862</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20">
-        <v>62</v>
-      </c>
-      <c r="C20">
-        <v>42</v>
-      </c>
-      <c r="D20">
-        <v>20</v>
-      </c>
-      <c r="E20">
-        <v>1.5009069086595199</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="B21">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="C21">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="D21">
-        <v>20</v>
+        <v>-44</v>
       </c>
       <c r="E21">
-        <v>1.5009069086595199</v>
+        <v>-2.93457815290631</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E21" xr:uid="{00000000-0001-0000-0200-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E21">
+      <sortCondition descending="1" ref="E1:E21"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1641,9 +1660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1672,53 +1689,53 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="B2">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="C2">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="D2">
-        <v>-16</v>
+        <v>24</v>
       </c>
       <c r="E2">
-        <v>-1.46560502354776</v>
+        <v>2.2687980698196402</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B3">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="D3">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E3">
-        <v>1.0551170644752399</v>
+        <v>2.1754379924854601</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B4">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="C4">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D4">
-        <v>-19</v>
+        <v>19</v>
       </c>
       <c r="E4">
-        <v>-1.7456852555503199</v>
+        <v>1.8019976831487201</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1740,172 +1757,172 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="B6">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="C6">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D6">
-        <v>-15</v>
+        <v>16</v>
       </c>
       <c r="E6">
-        <v>-1.37224494621358</v>
+        <v>1.5219174511461599</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="B7">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="C7">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D7">
-        <v>-12</v>
+        <v>14</v>
       </c>
       <c r="E7">
-        <v>-1.09216471421102</v>
+        <v>1.3351972964777901</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="B8">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C8">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="D8">
-        <v>-22</v>
+        <v>12</v>
       </c>
       <c r="E8">
-        <v>-2.0257654875528801</v>
+        <v>1.14847714180942</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B9">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="C9">
-        <v>65</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>-33</v>
+        <v>11</v>
       </c>
       <c r="E9">
-        <v>-3.05272633822891</v>
+        <v>1.0551170644752399</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="B10">
+        <v>47</v>
+      </c>
+      <c r="C10">
         <v>36</v>
       </c>
-      <c r="C10">
-        <v>52</v>
-      </c>
       <c r="D10">
-        <v>-16</v>
+        <v>11</v>
       </c>
       <c r="E10">
-        <v>-1.46560502354776</v>
+        <v>1.0551170644752399</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B11">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C11">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D11">
-        <v>12</v>
+        <v>-12</v>
       </c>
       <c r="E11">
-        <v>1.14847714180942</v>
+        <v>-1.09216471421102</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B12">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C12">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="D12">
-        <v>19</v>
+        <v>-14</v>
       </c>
       <c r="E12">
-        <v>1.8019976831487201</v>
+        <v>-1.2788848688793899</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="B13">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C13">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="D13">
-        <v>-14</v>
+        <v>-15</v>
       </c>
       <c r="E13">
-        <v>-1.2788848688793899</v>
+        <v>-1.37224494621358</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="B14">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="C14">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D14">
-        <v>11</v>
+        <v>-16</v>
       </c>
       <c r="E14">
-        <v>1.0551170644752399</v>
+        <v>-1.46560502354776</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B15">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C15">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="D15">
-        <v>14</v>
+        <v>-16</v>
       </c>
       <c r="E15">
-        <v>1.3351972964777901</v>
+        <v>-1.46560502354776</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1927,57 +1944,62 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B17">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="C17">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D17">
-        <v>23</v>
+        <v>-19</v>
       </c>
       <c r="E17">
-        <v>2.1754379924854601</v>
+        <v>-1.7456852555503199</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B18">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="C18">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D18">
-        <v>16</v>
+        <v>-22</v>
       </c>
       <c r="E18">
-        <v>1.5219174511461599</v>
+        <v>-2.0257654875528801</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B19">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="C19">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="D19">
-        <v>24</v>
+        <v>-33</v>
       </c>
       <c r="E19">
-        <v>2.2687980698196402</v>
+        <v>-3.05272633822891</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E19" xr:uid="{00000000-0001-0000-0300-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E19">
+      <sortCondition descending="1" ref="E1:E19"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>